<commit_message>
final status of REF Dispatcher
</commit_message>
<xml_diff>
--- a/YAS_Dispatcher/Data/Config.xlsx
+++ b/YAS_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashen\Desktop\Revature\YoutubeAutomationSuite\YAS_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1DBBE5-B7AE-4BFA-B546-A6BA413888D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB0229-14FE-4DA1-970D-1856878E9E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2787,7 +2787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Dispatcher Complete w/o REF (#56)
</commit_message>
<xml_diff>
--- a/YAS_Dispatcher/Data/Config.xlsx
+++ b/YAS_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashen\Desktop\Revature\YoutubeAutomationSuite\YAS_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1DBBE5-B7AE-4BFA-B546-A6BA413888D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB0229-14FE-4DA1-970D-1856878E9E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2787,7 +2787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>